<commit_message>
updated curve mesh with ETA_VALUES
</commit_message>
<xml_diff>
--- a/Sandia_blade_data.xlsx
+++ b/Sandia_blade_data.xlsx
@@ -1347,7 +1347,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1357,6 +1357,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1589,8 +1595,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10219,9 +10225,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V9" sqref="V9:V32"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
corrected shear web height when root buildup has nonzero thickness
</commit_message>
<xml_diff>
--- a/Sandia_blade_data.xlsx
+++ b/Sandia_blade_data.xlsx
@@ -1574,6 +1574,8 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1595,8 +1597,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2119,11 +2119,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115466624"/>
-        <c:axId val="115468544"/>
+        <c:axId val="83534208"/>
+        <c:axId val="83536128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115466624"/>
+        <c:axId val="83534208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2162,12 +2162,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115468544"/>
+        <c:crossAx val="83536128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115468544"/>
+        <c:axId val="83536128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2205,7 +2205,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115466624"/>
+        <c:crossAx val="83534208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2525,11 +2525,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115504640"/>
-        <c:axId val="115507200"/>
+        <c:axId val="92669440"/>
+        <c:axId val="92672000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115504640"/>
+        <c:axId val="92669440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2596,12 +2596,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115507200"/>
+        <c:crossAx val="92672000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115507200"/>
+        <c:axId val="92672000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2657,7 +2657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115504640"/>
+        <c:crossAx val="92669440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1"/>
@@ -3127,11 +3127,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43652608"/>
-        <c:axId val="43654528"/>
+        <c:axId val="92542464"/>
+        <c:axId val="92544384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43652608"/>
+        <c:axId val="92542464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3171,12 +3171,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43654528"/>
+        <c:crossAx val="92544384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43654528"/>
+        <c:axId val="92544384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3215,7 +3215,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43652608"/>
+        <c:crossAx val="92542464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3535,11 +3535,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43678336"/>
-        <c:axId val="43693184"/>
+        <c:axId val="92568192"/>
+        <c:axId val="92583040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43678336"/>
+        <c:axId val="92568192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3576,7 +3576,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -3607,12 +3606,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43693184"/>
+        <c:crossAx val="92583040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43693184"/>
+        <c:axId val="92583040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3638,7 +3637,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -3669,7 +3667,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43678336"/>
+        <c:crossAx val="92568192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1"/>
@@ -3941,8 +3939,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43737088"/>
-        <c:axId val="43739008"/>
+        <c:axId val="92630400"/>
+        <c:axId val="92632576"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4134,11 +4132,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43747200"/>
-        <c:axId val="43745280"/>
+        <c:axId val="92640768"/>
+        <c:axId val="92634496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43737088"/>
+        <c:axId val="92630400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -4205,12 +4203,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43739008"/>
+        <c:crossAx val="92632576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43739008"/>
+        <c:axId val="92632576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4274,12 +4272,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43737088"/>
+        <c:crossAx val="92630400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43745280"/>
+        <c:axId val="92634496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4353,13 +4351,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43747200"/>
+        <c:crossAx val="92640768"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2.0000000000000004E-2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43747200"/>
+        <c:axId val="92640768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4369,7 +4367,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43745280"/>
+        <c:crossAx val="92634496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4636,11 +4634,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43880832"/>
-        <c:axId val="43883136"/>
+        <c:axId val="92659712"/>
+        <c:axId val="92662016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43880832"/>
+        <c:axId val="92659712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -4677,7 +4675,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -4708,12 +4705,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43883136"/>
+        <c:crossAx val="92662016"/>
         <c:crossesAt val="-5.0000000000000012E-4"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43883136"/>
+        <c:axId val="92662016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4789,7 +4786,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43880832"/>
+        <c:crossAx val="92659712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5165,11 +5162,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44492672"/>
-        <c:axId val="44070016"/>
+        <c:axId val="95802880"/>
+        <c:axId val="95519488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44492672"/>
+        <c:axId val="95802880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.25"/>
@@ -5214,12 +5211,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44070016"/>
+        <c:crossAx val="95519488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44070016"/>
+        <c:axId val="95519488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5275,7 +5272,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44492672"/>
+        <c:crossAx val="95802880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5646,11 +5643,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44093824"/>
-        <c:axId val="44096896"/>
+        <c:axId val="95543296"/>
+        <c:axId val="95546368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44093824"/>
+        <c:axId val="95543296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0000000000000012E-2"/>
@@ -5696,12 +5693,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44096896"/>
+        <c:crossAx val="95546368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44096896"/>
+        <c:axId val="95546368"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5758,7 +5755,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44093824"/>
+        <c:crossAx val="95543296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7176,10 +7173,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="96" t="s">
         <v>56</v>
       </c>
       <c r="C1" s="25" t="s">
@@ -7199,8 +7196,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="94"/>
-      <c r="B2" s="94"/>
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
       <c r="C2" s="22" t="s">
         <v>49</v>
       </c>
@@ -7218,7 +7215,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="95"/>
+      <c r="A3" s="97"/>
       <c r="B3" s="19" t="s">
         <v>55</v>
       </c>
@@ -7956,16 +7953,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K1" s="96" t="s">
+      <c r="K1" s="98" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
       <c r="N1" s="41"/>
-      <c r="O1" s="96" t="s">
+      <c r="O1" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="96"/>
+      <c r="P1" s="98"/>
       <c r="Q1" s="42"/>
     </row>
     <row r="2" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -9912,48 +9909,48 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="100" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="100" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="98" t="s">
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="97" t="s">
+      <c r="M2" s="99" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="99"/>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="96" t="s">
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96" t="s">
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96" t="s">
+      <c r="I3" s="98"/>
+      <c r="J3" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="96"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="94"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="96"/>
     </row>
     <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
@@ -9992,7 +9989,7 @@
       <c r="L4" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="95"/>
+      <c r="M4" s="97"/>
     </row>
     <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -10225,9 +10222,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="A32:XFD32"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P9" sqref="P9:P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10257,16 +10254,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="K1" s="96" t="s">
+      <c r="K1" s="98" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
       <c r="N1" s="41"/>
-      <c r="O1" s="96" t="s">
+      <c r="O1" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="96"/>
+      <c r="P1" s="98"/>
       <c r="Q1" s="42"/>
     </row>
     <row r="2" spans="1:26" ht="60" x14ac:dyDescent="0.25">
@@ -10707,8 +10704,8 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P9" s="32">
-        <f t="shared" ref="P9:P32" si="3">D9*I9</f>
-        <v>5.3923519999999998</v>
+        <f>D9*I9-2*M9</f>
+        <v>5.2663519999999995</v>
       </c>
       <c r="Q9" s="3"/>
       <c r="R9" s="9" t="s">
@@ -10718,19 +10715,19 @@
         <v>91</v>
       </c>
       <c r="T9" s="7">
-        <f t="shared" ref="T9:T32" si="4">C9-$C$9</f>
+        <f t="shared" ref="T9:T32" si="3">C9-$C$9</f>
         <v>0</v>
       </c>
       <c r="U9" s="92">
         <f>T9/$T$32</f>
         <v>0</v>
       </c>
-      <c r="V9" s="101">
+      <c r="V9" s="94">
         <f>U9</f>
         <v>0</v>
       </c>
       <c r="W9" s="3">
-        <f t="shared" ref="W9:W32" si="5">L9+M9</f>
+        <f t="shared" ref="W9:W32" si="4">L9+M9</f>
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="X9" s="3">
@@ -10764,7 +10761,7 @@
         <v>13.308</v>
       </c>
       <c r="F10" s="56">
-        <f t="shared" ref="F10:F32" si="6">RADIANS(E10)</f>
+        <f t="shared" ref="F10:F32" si="5">RADIANS(E10)</f>
         <v>0.23226841685540536</v>
       </c>
       <c r="G10" s="57">
@@ -10795,8 +10792,8 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P10" s="32">
-        <f t="shared" si="3"/>
-        <v>5.3751750000000005</v>
+        <f>D10*I10-2*M10</f>
+        <v>5.2651750000000002</v>
       </c>
       <c r="Q10" s="3"/>
       <c r="R10" s="9"/>
@@ -10804,27 +10801,27 @@
         <v>91</v>
       </c>
       <c r="T10" s="7">
+        <f t="shared" si="3"/>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="U10" s="92">
+        <f t="shared" ref="U10:U32" si="6">T10/$T$32</f>
+        <v>2.1762785636561502E-3</v>
+      </c>
+      <c r="V10" s="94">
+        <f t="shared" ref="V10:V21" si="7">U10</f>
+        <v>2.1762785636561502E-3</v>
+      </c>
+      <c r="W10" s="3">
         <f t="shared" si="4"/>
-        <v>0.20000000000000018</v>
-      </c>
-      <c r="U10" s="92">
-        <f t="shared" ref="U10:U32" si="7">T10/$T$32</f>
-        <v>2.1762785636561502E-3</v>
-      </c>
-      <c r="V10" s="101">
-        <f t="shared" ref="V10:V21" si="8">U10</f>
-        <v>2.1762785636561502E-3</v>
-      </c>
-      <c r="W10" s="3">
-        <f t="shared" si="5"/>
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="X10" s="3">
-        <f t="shared" ref="X10:X32" si="9">W10</f>
+        <f t="shared" ref="X10:X32" si="8">W10</f>
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="Y10">
-        <f t="shared" ref="Y10:Y32" si="10">(F10-F9)/(T10-T9)</f>
+        <f t="shared" ref="Y10:Y32" si="9">(F10-F9)/(T10-T9)</f>
         <v>0</v>
       </c>
       <c r="Z10" s="85">
@@ -10852,7 +10849,7 @@
         <v>13.308</v>
       </c>
       <c r="F11" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.23226841685540536</v>
       </c>
       <c r="G11" s="57">
@@ -10883,8 +10880,8 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P11" s="32">
-        <f t="shared" si="3"/>
-        <v>5.0887199999999995</v>
+        <f t="shared" ref="P11:P21" si="10">D11*I11-2*M11</f>
+        <v>5.0087199999999994</v>
       </c>
       <c r="Q11" s="3"/>
       <c r="R11" s="9"/>
@@ -10892,27 +10889,27 @@
         <v>91</v>
       </c>
       <c r="T11" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2.3000000000000003</v>
       </c>
       <c r="U11" s="92">
+        <f t="shared" si="6"/>
+        <v>2.5027203482045707E-2</v>
+      </c>
+      <c r="V11" s="94">
         <f t="shared" si="7"/>
         <v>2.5027203482045707E-2</v>
       </c>
-      <c r="V11" s="101">
+      <c r="W11" s="3">
+        <f t="shared" si="4"/>
+        <v>0.06</v>
+      </c>
+      <c r="X11" s="3">
         <f t="shared" si="8"/>
-        <v>2.5027203482045707E-2</v>
-      </c>
-      <c r="W11" s="3">
-        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
-      <c r="X11" s="3">
+      <c r="Y11">
         <f t="shared" si="9"/>
-        <v>0.06</v>
-      </c>
-      <c r="Y11">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z11" s="85">
@@ -10940,7 +10937,7 @@
         <v>13.308</v>
       </c>
       <c r="F12" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.23226841685540536</v>
       </c>
       <c r="G12" s="57">
@@ -10971,8 +10968,8 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P12" s="32">
-        <f t="shared" si="3"/>
-        <v>4.7910400000000006</v>
+        <f t="shared" si="10"/>
+        <v>4.7410400000000008</v>
       </c>
       <c r="Q12" s="3"/>
       <c r="R12" s="9"/>
@@ -10980,27 +10977,27 @@
         <v>91</v>
       </c>
       <c r="T12" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="U12" s="92">
+        <f t="shared" si="6"/>
+        <v>4.7878128400435267E-2</v>
+      </c>
+      <c r="V12" s="94">
         <f t="shared" si="7"/>
         <v>4.7878128400435267E-2</v>
       </c>
-      <c r="V12" s="101">
+      <c r="W12" s="3">
+        <f t="shared" si="4"/>
+        <v>5.5E-2</v>
+      </c>
+      <c r="X12" s="3">
         <f t="shared" si="8"/>
-        <v>4.7878128400435267E-2</v>
-      </c>
-      <c r="W12" s="3">
-        <f t="shared" si="5"/>
         <v>5.5E-2</v>
       </c>
-      <c r="X12" s="3">
+      <c r="Y12">
         <f t="shared" si="9"/>
-        <v>5.5E-2</v>
-      </c>
-      <c r="Y12">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z12" s="85">
@@ -11028,7 +11025,7 @@
         <v>13.308</v>
       </c>
       <c r="F13" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.23226841685540536</v>
       </c>
       <c r="G13" s="57">
@@ -11059,8 +11056,8 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P13" s="32">
-        <f t="shared" si="3"/>
-        <v>4.4546800000000006</v>
+        <f t="shared" si="10"/>
+        <v>4.4246800000000004</v>
       </c>
       <c r="Q13" s="3"/>
       <c r="R13" s="9" t="s">
@@ -11070,27 +11067,27 @@
         <v>91</v>
       </c>
       <c r="T13" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6.5</v>
       </c>
       <c r="U13" s="92">
+        <f t="shared" si="6"/>
+        <v>7.0729053318824814E-2</v>
+      </c>
+      <c r="V13" s="94">
         <f t="shared" si="7"/>
         <v>7.0729053318824814E-2</v>
       </c>
-      <c r="V13" s="101">
+      <c r="W13" s="3">
+        <f t="shared" si="4"/>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="X13" s="3">
         <f t="shared" si="8"/>
-        <v>7.0729053318824814E-2</v>
-      </c>
-      <c r="W13" s="3">
-        <f t="shared" si="5"/>
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="X13" s="3">
+      <c r="Y13">
         <f t="shared" si="9"/>
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="Y13">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z13" s="85">
@@ -11118,7 +11115,7 @@
         <v>13.308</v>
       </c>
       <c r="F14" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.23226841685540536</v>
       </c>
       <c r="G14" s="57">
@@ -11149,8 +11146,8 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P14" s="32">
-        <f t="shared" si="3"/>
-        <v>4.101</v>
+        <f t="shared" si="10"/>
+        <v>4.0910000000000002</v>
       </c>
       <c r="Q14" s="3"/>
       <c r="R14" s="9"/>
@@ -11158,27 +11155,27 @@
         <v>91</v>
       </c>
       <c r="T14" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="U14" s="92">
+        <f t="shared" si="6"/>
+        <v>9.7932535364526674E-2</v>
+      </c>
+      <c r="V14" s="94">
         <f t="shared" si="7"/>
         <v>9.7932535364526674E-2</v>
       </c>
-      <c r="V14" s="101">
+      <c r="W14" s="3">
+        <f t="shared" si="4"/>
+        <v>7.3000000000000009E-2</v>
+      </c>
+      <c r="X14" s="3">
         <f t="shared" si="8"/>
-        <v>9.7932535364526674E-2</v>
-      </c>
-      <c r="W14" s="3">
-        <f t="shared" si="5"/>
         <v>7.3000000000000009E-2</v>
       </c>
-      <c r="X14" s="3">
+      <c r="Y14">
         <f t="shared" si="9"/>
-        <v>7.3000000000000009E-2</v>
-      </c>
-      <c r="Y14">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z14" s="85">
@@ -11206,7 +11203,7 @@
         <v>13.308</v>
       </c>
       <c r="F15" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.23226841685540536</v>
       </c>
       <c r="G15" s="57">
@@ -11236,7 +11233,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P15" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>3.6796500000000001</v>
       </c>
       <c r="Q15" s="3"/>
@@ -11247,19 +11244,19 @@
         <v>91</v>
       </c>
       <c r="T15" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>12.2</v>
       </c>
       <c r="U15" s="92">
+        <f t="shared" si="6"/>
+        <v>0.13275299238302504</v>
+      </c>
+      <c r="V15" s="94">
         <f t="shared" si="7"/>
         <v>0.13275299238302504</v>
       </c>
-      <c r="V15" s="101">
-        <f t="shared" si="8"/>
-        <v>0.13275299238302504</v>
-      </c>
       <c r="W15" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>9.4E-2</v>
       </c>
       <c r="X15" s="3">
@@ -11267,7 +11264,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Z15" s="85">
@@ -11295,7 +11292,7 @@
         <v>13.177</v>
       </c>
       <c r="F16" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.22998203553529278</v>
       </c>
       <c r="G16" s="57">
@@ -11325,7 +11322,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P16" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>3.4798799999999996</v>
       </c>
       <c r="Q16" s="3"/>
@@ -11334,19 +11331,19 @@
         <v>91</v>
       </c>
       <c r="T16" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>13.9</v>
       </c>
       <c r="U16" s="92">
+        <f t="shared" si="6"/>
+        <v>0.15125136017410229</v>
+      </c>
+      <c r="V16" s="94">
         <f t="shared" si="7"/>
         <v>0.15125136017410229</v>
       </c>
-      <c r="V16" s="101">
-        <f t="shared" si="8"/>
-        <v>0.15125136017410229</v>
-      </c>
       <c r="W16" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.111</v>
       </c>
       <c r="X16" s="3">
@@ -11354,7 +11351,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>-1.3449301883015163E-3</v>
       </c>
       <c r="Z16" s="85">
@@ -11382,7 +11379,7 @@
         <v>13.045999999999999</v>
       </c>
       <c r="F17" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.22769565421518023</v>
       </c>
       <c r="G17" s="57">
@@ -11412,7 +11409,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P17" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>3.2851199999999996</v>
       </c>
       <c r="Q17" s="3"/>
@@ -11421,19 +11418,19 @@
         <v>91</v>
       </c>
       <c r="T17" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15.499999999999998</v>
       </c>
       <c r="U17" s="92">
         <f>T17/$T$32</f>
         <v>0.16866158868335146</v>
       </c>
-      <c r="V17" s="101">
-        <f t="shared" si="8"/>
+      <c r="V17" s="94">
+        <f t="shared" si="7"/>
         <v>0.16866158868335146</v>
       </c>
       <c r="W17" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.11899999999999999</v>
       </c>
       <c r="X17" s="3">
@@ -11441,7 +11438,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>-1.4289883250703467E-3</v>
       </c>
       <c r="Z17" s="85">
@@ -11469,7 +11466,7 @@
         <v>12.914999999999999</v>
       </c>
       <c r="F18" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.22540927289506765</v>
       </c>
       <c r="G18" s="57">
@@ -11499,7 +11496,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P18" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>3.0893400000000004</v>
       </c>
       <c r="Q18" s="3"/>
@@ -11510,19 +11507,19 @@
         <v>91</v>
       </c>
       <c r="T18" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>17.100000000000001</v>
       </c>
       <c r="U18" s="92">
+        <f t="shared" si="6"/>
+        <v>0.18607181719260069</v>
+      </c>
+      <c r="V18" s="94">
         <f t="shared" si="7"/>
         <v>0.18607181719260069</v>
       </c>
-      <c r="V18" s="101">
-        <f t="shared" si="8"/>
-        <v>0.18607181719260069</v>
-      </c>
       <c r="W18" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.13600000000000001</v>
       </c>
       <c r="X18" s="3">
@@ -11530,7 +11527,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>-1.4289883250703593E-3</v>
       </c>
       <c r="Z18" s="85">
@@ -11558,7 +11555,7 @@
         <v>12.132999999999999</v>
       </c>
       <c r="F19" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.21176079814447199</v>
       </c>
       <c r="G19" s="57">
@@ -11588,7 +11585,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P19" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>2.8822999999999999</v>
       </c>
       <c r="Q19" s="3"/>
@@ -11597,19 +11594,19 @@
         <v>91</v>
       </c>
       <c r="T19" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>19.8</v>
       </c>
       <c r="U19" s="92">
+        <f t="shared" si="6"/>
+        <v>0.21545157780195867</v>
+      </c>
+      <c r="V19" s="94">
         <f t="shared" si="7"/>
         <v>0.21545157780195867</v>
       </c>
-      <c r="V19" s="101">
-        <f t="shared" si="8"/>
-        <v>0.21545157780195867</v>
-      </c>
       <c r="W19" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.13600000000000001</v>
       </c>
       <c r="X19" s="3">
@@ -11617,7 +11614,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>-5.0549906483687655E-3</v>
       </c>
       <c r="Z19" s="85">
@@ -11645,7 +11642,7 @@
         <v>11.35</v>
       </c>
       <c r="F20" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.1980948701013564</v>
       </c>
       <c r="G20" s="57">
@@ -11675,7 +11672,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P20" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>2.6956799999999999</v>
       </c>
       <c r="Q20" s="3"/>
@@ -11684,19 +11681,19 @@
         <v>91</v>
       </c>
       <c r="T20" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>22.5</v>
       </c>
       <c r="U20" s="92">
+        <f t="shared" si="6"/>
+        <v>0.24483133841131668</v>
+      </c>
+      <c r="V20" s="94">
         <f t="shared" si="7"/>
         <v>0.24483133841131668</v>
       </c>
-      <c r="V20" s="101">
-        <f t="shared" si="8"/>
-        <v>0.24483133841131668</v>
-      </c>
       <c r="W20" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.13600000000000001</v>
       </c>
       <c r="X20" s="3">
@@ -11704,7 +11701,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>-5.0614548307835521E-3</v>
       </c>
       <c r="Z20" s="85">
@@ -11732,7 +11729,7 @@
         <v>10.568</v>
       </c>
       <c r="F21" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.18444639535076074</v>
       </c>
       <c r="G21" s="57">
@@ -11762,7 +11759,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P21" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>2.4979800000000005</v>
       </c>
       <c r="Q21" s="3"/>
@@ -11771,19 +11768,19 @@
         <v>91</v>
       </c>
       <c r="T21" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>25.200000000000003</v>
       </c>
       <c r="U21" s="92">
+        <f t="shared" si="6"/>
+        <v>0.2742110990206747</v>
+      </c>
+      <c r="V21" s="94">
         <f t="shared" si="7"/>
         <v>0.2742110990206747</v>
       </c>
-      <c r="V21" s="101">
-        <f t="shared" si="8"/>
-        <v>0.2742110990206747</v>
-      </c>
       <c r="W21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.128</v>
       </c>
       <c r="X21" s="3">
@@ -11791,7 +11788,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>-5.0549906483687585E-3</v>
       </c>
       <c r="Z21" s="85">
@@ -11819,7 +11816,7 @@
         <v>9.1660000000000004</v>
       </c>
       <c r="F22" s="73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.15997687923780024</v>
       </c>
       <c r="G22" s="74">
@@ -11850,7 +11847,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P22" s="79">
-        <f t="shared" si="3"/>
+        <f>D22*I22-2*M22</f>
         <v>2.0768999999999997</v>
       </c>
       <c r="Q22" s="82"/>
@@ -11859,19 +11856,19 @@
         <v>91</v>
       </c>
       <c r="T22" s="90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>33.4</v>
       </c>
       <c r="U22" s="93">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.36343852013057676</v>
       </c>
-      <c r="V22" s="102">
+      <c r="V22" s="95">
         <f>U22</f>
         <v>0.36343852013057676</v>
       </c>
       <c r="W22" s="82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.11899999999999999</v>
       </c>
       <c r="X22" s="82">
@@ -11879,7 +11876,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="Y22" s="81">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>-2.984087330848843E-3</v>
       </c>
       <c r="Z22" s="91">
@@ -11907,7 +11904,7 @@
         <v>7.6879999999999997</v>
       </c>
       <c r="F23" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.13418091289332404</v>
       </c>
       <c r="G23" s="57">
@@ -11937,7 +11934,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P23" s="32">
-        <f t="shared" si="3"/>
+        <f>D23*I23-2*M23</f>
         <v>1.67154</v>
       </c>
       <c r="Q23" s="3"/>
@@ -11946,19 +11943,19 @@
         <v>92</v>
       </c>
       <c r="T23" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>41.5</v>
       </c>
       <c r="U23" s="92">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.45157780195865077</v>
       </c>
-      <c r="V23" s="101">
+      <c r="V23" s="94">
         <f>U23</f>
         <v>0.45157780195865077</v>
       </c>
       <c r="W23" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.111</v>
       </c>
       <c r="X23" s="3">
@@ -11966,7 +11963,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>-3.1846872030217525E-3</v>
       </c>
       <c r="Z23" s="85">
@@ -11994,7 +11991,7 @@
         <v>6.18</v>
       </c>
       <c r="F24" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.10786134777324956</v>
       </c>
       <c r="G24" s="57">
@@ -12024,7 +12021,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P24" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="P24:P32" si="13">D24*I24-2*M24</f>
         <v>1.3604500000000002</v>
       </c>
       <c r="Q24" s="3"/>
@@ -12033,19 +12030,19 @@
         <v>92</v>
       </c>
       <c r="T24" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>49.6</v>
       </c>
       <c r="U24" s="92">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.53971708378672478</v>
       </c>
-      <c r="V24" s="101">
+      <c r="V24" s="94">
         <f>U24</f>
         <v>0.53971708378672478</v>
       </c>
       <c r="W24" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.10199999999999999</v>
       </c>
       <c r="X24" s="3">
@@ -12053,7 +12050,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="Y24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>-3.2493290271696884E-3</v>
       </c>
       <c r="Z24" s="85">
@@ -12081,7 +12078,7 @@
         <v>4.7430000000000003</v>
       </c>
       <c r="F25" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>8.2780966422091054E-2</v>
       </c>
       <c r="G25" s="57">
@@ -12111,7 +12108,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P25" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>1.13757</v>
       </c>
       <c r="Q25" s="3"/>
@@ -12122,27 +12119,27 @@
         <v>92</v>
       </c>
       <c r="T25" s="7">
+        <f t="shared" si="3"/>
+        <v>57.8</v>
+      </c>
+      <c r="U25" s="92">
+        <f t="shared" si="6"/>
+        <v>0.62894450489662679</v>
+      </c>
+      <c r="V25" s="94">
+        <f t="shared" ref="V25:V32" si="14">U25</f>
+        <v>0.62894450489662679</v>
+      </c>
+      <c r="W25" s="3">
         <f t="shared" si="4"/>
-        <v>57.8</v>
-      </c>
-      <c r="U25" s="92">
-        <f t="shared" si="7"/>
-        <v>0.62894450489662679</v>
-      </c>
-      <c r="V25" s="101">
-        <f t="shared" ref="V25:V32" si="13">U25</f>
-        <v>0.62894450489662679</v>
-      </c>
-      <c r="W25" s="3">
-        <f t="shared" si="5"/>
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="X25" s="3">
+        <f t="shared" si="8"/>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="Y25">
         <f t="shared" si="9"/>
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="Y25">
-        <f t="shared" si="10"/>
         <v>-3.0585830916046971E-3</v>
       </c>
       <c r="Z25" s="85">
@@ -12170,7 +12167,7 @@
         <v>3.633</v>
       </c>
       <c r="F26" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>6.3407811724953994E-2</v>
       </c>
       <c r="G26" s="57">
@@ -12200,7 +12197,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P26" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0.95361000000000007</v>
       </c>
       <c r="Q26" s="3"/>
@@ -12209,27 +12206,27 @@
         <v>92</v>
       </c>
       <c r="T26" s="7">
+        <f t="shared" si="3"/>
+        <v>64.3</v>
+      </c>
+      <c r="U26" s="92">
+        <f t="shared" si="6"/>
+        <v>0.69967355821545163</v>
+      </c>
+      <c r="V26" s="94">
+        <f t="shared" si="14"/>
+        <v>0.69967355821545163</v>
+      </c>
+      <c r="W26" s="3">
         <f t="shared" si="4"/>
-        <v>64.3</v>
-      </c>
-      <c r="U26" s="92">
-        <f t="shared" si="7"/>
-        <v>0.69967355821545163</v>
-      </c>
-      <c r="V26" s="101">
-        <f t="shared" si="13"/>
-        <v>0.69967355821545163</v>
-      </c>
-      <c r="W26" s="3">
-        <f t="shared" si="5"/>
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="X26" s="3">
+        <f t="shared" si="8"/>
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="Y26">
         <f t="shared" si="9"/>
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="Y26">
-        <f t="shared" si="10"/>
         <v>-2.9804853380210861E-3</v>
       </c>
       <c r="Z26" s="85">
@@ -12257,7 +12254,7 @@
         <v>3.383</v>
       </c>
       <c r="F27" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>5.9044488594968171E-2</v>
       </c>
       <c r="G27" s="57">
@@ -12287,7 +12284,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P27" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0.91020000000000001</v>
       </c>
       <c r="Q27" s="3"/>
@@ -12296,27 +12293,27 @@
         <v>92</v>
       </c>
       <c r="T27" s="7">
+        <f t="shared" si="3"/>
+        <v>65.900000000000006</v>
+      </c>
+      <c r="U27" s="92">
+        <f t="shared" si="6"/>
+        <v>0.71708378672470086</v>
+      </c>
+      <c r="V27" s="94">
+        <f t="shared" si="14"/>
+        <v>0.71708378672470086</v>
+      </c>
+      <c r="W27" s="3">
         <f t="shared" si="4"/>
-        <v>65.900000000000006</v>
-      </c>
-      <c r="U27" s="92">
-        <f t="shared" si="7"/>
-        <v>0.71708378672470086</v>
-      </c>
-      <c r="V27" s="101">
-        <f t="shared" si="13"/>
-        <v>0.71708378672470086</v>
-      </c>
-      <c r="W27" s="3">
-        <f t="shared" si="5"/>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="X27" s="3">
+        <f t="shared" si="8"/>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="Y27">
         <f t="shared" si="9"/>
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="Y27">
-        <f t="shared" si="10"/>
         <v>-2.7270769562411246E-3</v>
       </c>
       <c r="Z27" s="85">
@@ -12344,7 +12341,7 @@
         <v>2.7349999999999999</v>
       </c>
       <c r="F28" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4.7734755042044913E-2</v>
       </c>
       <c r="G28" s="57">
@@ -12374,7 +12371,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P28" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0.83178000000000007</v>
       </c>
       <c r="Q28" s="3"/>
@@ -12383,27 +12380,27 @@
         <v>92</v>
       </c>
       <c r="T28" s="7">
+        <f t="shared" si="3"/>
+        <v>70.8</v>
+      </c>
+      <c r="U28" s="92">
+        <f t="shared" si="6"/>
+        <v>0.77040261153427647</v>
+      </c>
+      <c r="V28" s="94">
+        <f t="shared" si="14"/>
+        <v>0.77040261153427647</v>
+      </c>
+      <c r="W28" s="3">
         <f t="shared" si="4"/>
-        <v>70.8</v>
-      </c>
-      <c r="U28" s="92">
-        <f t="shared" si="7"/>
-        <v>0.77040261153427647</v>
-      </c>
-      <c r="V28" s="101">
-        <f t="shared" si="13"/>
-        <v>0.77040261153427647</v>
-      </c>
-      <c r="W28" s="3">
-        <f t="shared" si="5"/>
         <v>4.7E-2</v>
       </c>
       <c r="X28" s="3">
+        <f t="shared" si="8"/>
+        <v>4.7E-2</v>
+      </c>
+      <c r="Y28">
         <f t="shared" si="9"/>
-        <v>4.7E-2</v>
-      </c>
-      <c r="Y28">
-        <f t="shared" si="10"/>
         <v>-2.3081088883516892E-3</v>
       </c>
       <c r="Z28" s="85">
@@ -12431,7 +12428,7 @@
         <v>2.3479999999999999</v>
       </c>
       <c r="F29" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4.0980330836826853E-2</v>
       </c>
       <c r="G29" s="57">
@@ -12461,7 +12458,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P29" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0.79595999999999989</v>
       </c>
       <c r="Q29" s="3"/>
@@ -12470,27 +12467,27 @@
         <v>92</v>
       </c>
       <c r="T29" s="7">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+      <c r="U29" s="92">
+        <f t="shared" si="6"/>
+        <v>0.80522306855277481</v>
+      </c>
+      <c r="V29" s="94">
+        <f t="shared" si="14"/>
+        <v>0.80522306855277481</v>
+      </c>
+      <c r="W29" s="3">
         <f t="shared" si="4"/>
-        <v>74</v>
-      </c>
-      <c r="U29" s="92">
-        <f t="shared" si="7"/>
-        <v>0.80522306855277481</v>
-      </c>
-      <c r="V29" s="101">
-        <f t="shared" si="13"/>
-        <v>0.80522306855277481</v>
-      </c>
-      <c r="W29" s="3">
-        <f t="shared" si="5"/>
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="X29" s="3">
+        <f t="shared" si="8"/>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="Y29">
         <f t="shared" si="9"/>
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="Y29">
-        <f t="shared" si="10"/>
         <v>-2.1107575641306419E-3</v>
       </c>
       <c r="Z29" s="85">
@@ -12518,7 +12515,7 @@
         <v>1.38</v>
       </c>
       <c r="F30" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4085543677521744E-2</v>
       </c>
       <c r="G30" s="57">
@@ -12548,7 +12545,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P30" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0.70649999999999991</v>
       </c>
       <c r="Q30" s="3"/>
@@ -12557,27 +12554,27 @@
         <v>92</v>
       </c>
       <c r="T30" s="7">
+        <f t="shared" si="3"/>
+        <v>82.199999999999989</v>
+      </c>
+      <c r="U30" s="92">
+        <f t="shared" si="6"/>
+        <v>0.89445048966267682</v>
+      </c>
+      <c r="V30" s="94">
+        <f t="shared" si="14"/>
+        <v>0.89445048966267682</v>
+      </c>
+      <c r="W30" s="3">
         <f t="shared" si="4"/>
-        <v>82.199999999999989</v>
-      </c>
-      <c r="U30" s="92">
-        <f t="shared" si="7"/>
-        <v>0.89445048966267682</v>
-      </c>
-      <c r="V30" s="101">
-        <f t="shared" si="13"/>
-        <v>0.89445048966267682</v>
-      </c>
-      <c r="W30" s="3">
-        <f t="shared" si="5"/>
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="X30" s="3">
+        <f t="shared" si="8"/>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="Y30">
         <f t="shared" si="9"/>
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="Y30">
-        <f t="shared" si="10"/>
         <v>-2.0603398974762357E-3</v>
       </c>
       <c r="Z30" s="85">
@@ -12605,7 +12602,7 @@
         <v>0.79900000000000004</v>
       </c>
       <c r="F31" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1.3945180723434694E-2</v>
       </c>
       <c r="G31" s="57">
@@ -12635,7 +12632,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P31" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0.65142</v>
       </c>
       <c r="Q31" s="3"/>
@@ -12644,27 +12641,27 @@
         <v>92</v>
       </c>
       <c r="T31" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>87</v>
       </c>
       <c r="U31" s="92">
         <f>T31/$T$32</f>
         <v>0.9466811751904245</v>
       </c>
-      <c r="V31" s="101">
-        <f t="shared" si="13"/>
+      <c r="V31" s="94">
+        <f t="shared" si="14"/>
         <v>0.9466811751904245</v>
       </c>
       <c r="W31" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="X31" s="3">
+        <f t="shared" si="8"/>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="Y31">
         <f t="shared" si="9"/>
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="Y31">
-        <f t="shared" si="10"/>
         <v>-2.1125756154347971E-3</v>
       </c>
       <c r="Z31" s="85">
@@ -12692,7 +12689,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="F32" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4.8869219055841231E-3</v>
       </c>
       <c r="G32" s="57">
@@ -12722,7 +12719,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P32" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>0.50831999999999999</v>
       </c>
       <c r="Q32" s="3"/>
@@ -12733,27 +12730,27 @@
         <v>92</v>
       </c>
       <c r="T32" s="7">
+        <f t="shared" si="3"/>
+        <v>91.899999999999991</v>
+      </c>
+      <c r="U32" s="92">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V32" s="94">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="W32" s="3">
         <f t="shared" si="4"/>
-        <v>91.899999999999991</v>
-      </c>
-      <c r="U32" s="92">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="V32" s="101">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="W32" s="3">
-        <f t="shared" si="5"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="X32" s="3">
+        <f t="shared" si="8"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="Y32">
         <f t="shared" si="9"/>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="Y32">
-        <f t="shared" si="10"/>
         <v>-1.8486242485409362E-3</v>
       </c>
       <c r="Z32" s="85">
@@ -12830,7 +12827,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="F34" s="36">
-        <f t="shared" ref="F34:F35" si="14">RADIANS(E34)</f>
+        <f t="shared" ref="F34:F35" si="15">RADIANS(E34)</f>
         <v>2.4434609527920616E-3</v>
       </c>
       <c r="G34" s="47">
@@ -12879,7 +12876,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F35" s="36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.2217304763960308E-3</v>
       </c>
       <c r="G35" s="47">
@@ -13007,16 +13004,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K1" s="96" t="s">
+      <c r="K1" s="98" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
       <c r="N1" s="41"/>
-      <c r="O1" s="96" t="s">
+      <c r="O1" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="96"/>
+      <c r="P1" s="98"/>
       <c r="Q1" s="42"/>
     </row>
     <row r="2" spans="1:19" ht="75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
can plot forces at spar stations
</commit_message>
<xml_diff>
--- a/Sandia_blade_data.xlsx
+++ b/Sandia_blade_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="24240" windowHeight="9465" tabRatio="793" firstSheet="1" activeTab="6"/>
@@ -459,7 +459,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="161">
   <si>
     <t>Station Number</t>
   </si>
@@ -1644,6 +1644,15 @@
       <t>j</t>
     </r>
   </si>
+  <si>
+    <t>I_x</t>
+  </si>
+  <si>
+    <t>I_x (outer)</t>
+  </si>
+  <si>
+    <t>I_x (inner)</t>
+  </si>
 </sst>
 </file>
 
@@ -2151,6 +2160,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -2165,12 +2180,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2946,11 +2955,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="106284160"/>
-        <c:axId val="106286080"/>
+        <c:axId val="43784832"/>
+        <c:axId val="43787008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106284160"/>
+        <c:axId val="43784832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2990,12 +2999,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106286080"/>
+        <c:crossAx val="43787008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106286080"/>
+        <c:axId val="43787008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3034,7 +3043,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106284160"/>
+        <c:crossAx val="43784832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3354,11 +3363,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="106326272"/>
-        <c:axId val="106332928"/>
+        <c:axId val="43806720"/>
+        <c:axId val="43809024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106326272"/>
+        <c:axId val="43806720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3426,12 +3435,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106332928"/>
+        <c:crossAx val="43809024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106332928"/>
+        <c:axId val="43809024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3488,7 +3497,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106326272"/>
+        <c:crossAx val="43806720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1"/>
@@ -3541,6 +3550,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3957,11 +3967,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="107993344"/>
-        <c:axId val="107999616"/>
+        <c:axId val="43868160"/>
+        <c:axId val="43870080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="107993344"/>
+        <c:axId val="43868160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3984,6 +3994,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -4000,12 +4011,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107999616"/>
+        <c:crossAx val="43870080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107999616"/>
+        <c:axId val="43870080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4027,6 +4038,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -4043,7 +4055,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107993344"/>
+        <c:crossAx val="43868160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4363,11 +4375,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="106847616"/>
-        <c:axId val="106866560"/>
+        <c:axId val="44094592"/>
+        <c:axId val="44096896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106847616"/>
+        <c:axId val="44094592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -4404,6 +4416,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -4434,12 +4447,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106866560"/>
+        <c:crossAx val="44096896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106866560"/>
+        <c:axId val="44096896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4465,6 +4478,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -4495,7 +4509,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106847616"/>
+        <c:crossAx val="44094592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1"/>
@@ -4767,8 +4781,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="107491712"/>
-        <c:axId val="107493632"/>
+        <c:axId val="44719488"/>
+        <c:axId val="44725760"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4960,11 +4974,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="107497728"/>
-        <c:axId val="107495808"/>
+        <c:axId val="44729856"/>
+        <c:axId val="44727680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="107491712"/>
+        <c:axId val="44719488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -5031,12 +5045,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107493632"/>
+        <c:crossAx val="44725760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107493632"/>
+        <c:axId val="44725760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5100,12 +5114,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107491712"/>
+        <c:crossAx val="44719488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107495808"/>
+        <c:axId val="44727680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5179,13 +5193,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107497728"/>
+        <c:crossAx val="44729856"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2.0000000000000004E-2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107497728"/>
+        <c:axId val="44729856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5195,7 +5209,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107495808"/>
+        <c:crossAx val="44727680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5462,11 +5476,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="107537152"/>
-        <c:axId val="107539456"/>
+        <c:axId val="44499328"/>
+        <c:axId val="44501632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="107537152"/>
+        <c:axId val="44499328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -5503,6 +5517,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -5533,12 +5548,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107539456"/>
+        <c:crossAx val="44501632"/>
         <c:crossesAt val="-5.0000000000000012E-4"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107539456"/>
+        <c:axId val="44501632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5614,7 +5629,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107537152"/>
+        <c:crossAx val="44499328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5990,11 +6005,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="107661568"/>
-        <c:axId val="108094976"/>
+        <c:axId val="44519808"/>
+        <c:axId val="44522880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="107661568"/>
+        <c:axId val="44519808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.25"/>
@@ -6021,6 +6036,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
@@ -6039,12 +6055,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108094976"/>
+        <c:crossAx val="44522880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108094976"/>
+        <c:axId val="44522880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6082,6 +6098,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
@@ -6100,7 +6117,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107661568"/>
+        <c:crossAx val="44519808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6471,11 +6488,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="108110592"/>
-        <c:axId val="108122112"/>
+        <c:axId val="44669184"/>
+        <c:axId val="44684800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108110592"/>
+        <c:axId val="44669184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0000000000000012E-2"/>
@@ -6503,6 +6520,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
@@ -6521,12 +6539,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108122112"/>
+        <c:crossAx val="44684800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108122112"/>
+        <c:axId val="44684800"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6565,6 +6583,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
@@ -6583,7 +6602,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108110592"/>
+        <c:crossAx val="44669184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9260,7 +9279,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="P10" s="32">
-        <f t="shared" ref="P9:P32" si="4">D10*I10</f>
+        <f t="shared" ref="P10:P32" si="4">D10*I10</f>
         <v>5.3751750000000005</v>
       </c>
       <c r="Q10" s="3"/>
@@ -14557,10 +14576,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+      <selection activeCell="V2" sqref="V2:V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14583,9 +14602,13 @@
     <col min="16" max="16" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="1.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="96" t="s">
         <v>101</v>
       </c>
@@ -14640,8 +14663,17 @@
       <c r="R1" s="96" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T1" s="96" t="s">
+        <v>159</v>
+      </c>
+      <c r="U1" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="V1" s="96" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -14696,8 +14728,20 @@
       <c r="R2" s="3">
         <v>5.7919999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T2" s="97">
+        <f>(1/12)*$G$2*(J2+2*H2)^3</f>
+        <v>21.842617349461332</v>
+      </c>
+      <c r="U2" s="97">
+        <f>(1/12)*$E$2*(J2-2*F2)^3</f>
+        <v>17.984728000000004</v>
+      </c>
+      <c r="V2" s="97">
+        <f>T2-U2</f>
+        <v>3.8578893494613276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -14752,8 +14796,20 @@
       <c r="R3" s="3">
         <v>5.8109999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T3" s="97">
+        <f t="shared" ref="T3:T26" si="0">(1/12)*$G$2*(J3+2*H3)^3</f>
+        <v>21.636670572916664</v>
+      </c>
+      <c r="U3" s="97">
+        <f t="shared" ref="U3:U25" si="1">(1/12)*$E$2*(J3-2*F3)^3</f>
+        <v>17.974433364875001</v>
+      </c>
+      <c r="V3" s="97">
+        <f t="shared" ref="V3:V25" si="2">T3-U3</f>
+        <v>3.6622372080416632</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -14808,8 +14864,20 @@
       <c r="R4" s="3">
         <v>6.0579999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T4" s="97">
+        <f t="shared" si="0"/>
+        <v>18.363369782347334</v>
+      </c>
+      <c r="U4" s="97">
+        <f t="shared" si="1"/>
+        <v>15.336173151125001</v>
+      </c>
+      <c r="V4" s="97">
+        <f t="shared" si="2"/>
+        <v>3.0271966312223331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -14864,8 +14932,20 @@
       <c r="R5" s="3">
         <v>6.3040000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T5" s="97">
+        <f t="shared" si="0"/>
+        <v>15.322637936825993</v>
+      </c>
+      <c r="U5" s="97">
+        <f t="shared" si="1"/>
+        <v>12.821119155125002</v>
+      </c>
+      <c r="V5" s="97">
+        <f t="shared" si="2"/>
+        <v>2.501518781700991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -14920,8 +15000,20 @@
       <c r="R6" s="3">
         <v>6.5510000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T6" s="97">
+        <f t="shared" si="0"/>
+        <v>12.319643828250001</v>
+      </c>
+      <c r="U6" s="97">
+        <f t="shared" si="1"/>
+        <v>10.098705783374996</v>
+      </c>
+      <c r="V6" s="97">
+        <f t="shared" si="2"/>
+        <v>2.2209380448750053</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -14976,8 +15068,20 @@
       <c r="R7" s="3">
         <v>6.835</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T7" s="97">
+        <f t="shared" si="0"/>
+        <v>9.610020960605997</v>
+      </c>
+      <c r="U7" s="97">
+        <f t="shared" si="1"/>
+        <v>7.7330261093750003</v>
+      </c>
+      <c r="V7" s="97">
+        <f t="shared" si="2"/>
+        <v>1.8769948512309966</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -15032,8 +15136,20 @@
       <c r="R8" s="3">
         <v>7.2149999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T8" s="97">
+        <f t="shared" si="0"/>
+        <v>6.9438204586666661</v>
+      </c>
+      <c r="U8" s="97">
+        <f t="shared" si="1"/>
+        <v>5.3227089359999997</v>
+      </c>
+      <c r="V8" s="97">
+        <f t="shared" si="2"/>
+        <v>1.6211115226666664</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -15088,8 +15204,20 @@
       <c r="R9" s="3">
         <v>7.4039999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T9" s="97">
+        <f t="shared" si="0"/>
+        <v>5.8720907519999992</v>
+      </c>
+      <c r="U9" s="97">
+        <f t="shared" si="1"/>
+        <v>4.3227811889999996</v>
+      </c>
+      <c r="V9" s="97">
+        <f t="shared" si="2"/>
+        <v>1.5493095629999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -15144,8 +15272,20 @@
       <c r="R10" s="3">
         <v>7.5519999999999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T10" s="97">
+        <f t="shared" si="0"/>
+        <v>4.93925159475</v>
+      </c>
+      <c r="U10" s="97">
+        <f t="shared" si="1"/>
+        <v>3.5361231028750004</v>
+      </c>
+      <c r="V10" s="97">
+        <f t="shared" si="2"/>
+        <v>1.4031284918749996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -15200,8 +15340,20 @@
       <c r="R11" s="3">
         <v>7.6280000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T11" s="97">
+        <f t="shared" si="0"/>
+        <v>4.1068491596806656</v>
+      </c>
+      <c r="U11" s="97">
+        <f t="shared" si="1"/>
+        <v>2.7942840641250006</v>
+      </c>
+      <c r="V11" s="97">
+        <f t="shared" si="2"/>
+        <v>1.3125650955556649</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -15256,8 +15408,20 @@
       <c r="R12" s="3">
         <v>7.585</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T12" s="97">
+        <f t="shared" si="0"/>
+        <v>3.3353157668746669</v>
+      </c>
+      <c r="U12" s="97">
+        <f t="shared" si="1"/>
+        <v>2.2224476250000009</v>
+      </c>
+      <c r="V12" s="97">
+        <f t="shared" si="2"/>
+        <v>1.112868141874666</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -15312,8 +15476,20 @@
       <c r="R13" s="3">
         <v>7.4880000000000004</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T13" s="97">
+        <f t="shared" si="0"/>
+        <v>2.7303271686826664</v>
+      </c>
+      <c r="U13" s="97">
+        <f t="shared" si="1"/>
+        <v>1.7803601280000008</v>
+      </c>
+      <c r="V13" s="97">
+        <f t="shared" si="2"/>
+        <v>0.94996704068266569</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -15368,8 +15544,20 @@
       <c r="R14" s="3">
         <v>7.3470000000000004</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T14" s="97">
+        <f t="shared" si="0"/>
+        <v>2.171862512218667</v>
+      </c>
+      <c r="U14" s="97">
+        <f t="shared" si="1"/>
+        <v>1.4086945609999999</v>
+      </c>
+      <c r="V14" s="97">
+        <f t="shared" si="2"/>
+        <v>0.7631679512186671</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -15424,8 +15612,20 @@
       <c r="R15" s="3">
         <v>6.923</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T15" s="97">
+        <f t="shared" si="0"/>
+        <v>1.2484309209313331</v>
+      </c>
+      <c r="U15" s="97">
+        <f t="shared" si="1"/>
+        <v>0.77741908987499997</v>
+      </c>
+      <c r="V15" s="97">
+        <f t="shared" si="2"/>
+        <v>0.47101183105633315</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -15480,8 +15680,20 @@
       <c r="R16" s="3">
         <v>6.4290000000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T16" s="97">
+        <f t="shared" si="0"/>
+        <v>0.65127415842133307</v>
+      </c>
+      <c r="U16" s="97">
+        <f t="shared" si="1"/>
+        <v>0.38107812499999999</v>
+      </c>
+      <c r="V16" s="97">
+        <f t="shared" si="2"/>
+        <v>0.27019603342133308</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -15536,8 +15748,20 @@
       <c r="R17" s="3">
         <v>5.915</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T17" s="97">
+        <f t="shared" si="0"/>
+        <v>0.3504868693333334</v>
+      </c>
+      <c r="U17" s="97">
+        <f t="shared" si="1"/>
+        <v>0.19310055200000009</v>
+      </c>
+      <c r="V17" s="97">
+        <f t="shared" si="2"/>
+        <v>0.1573863173333333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -15592,8 +15816,20 @@
       <c r="R18" s="3">
         <v>5.4169999999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T18" s="97">
+        <f t="shared" si="0"/>
+        <v>0.20534390336533326</v>
+      </c>
+      <c r="U18" s="97">
+        <f t="shared" si="1"/>
+        <v>0.11337990399999995</v>
+      </c>
+      <c r="V18" s="97">
+        <f t="shared" si="2"/>
+        <v>9.196399936533331E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -15648,8 +15884,20 @@
       <c r="R19" s="3">
         <v>5.0190000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T19" s="97">
+        <f t="shared" si="0"/>
+        <v>0.12097625918399996</v>
+      </c>
+      <c r="U19" s="97">
+        <f t="shared" si="1"/>
+        <v>6.8417928999999988E-2</v>
+      </c>
+      <c r="V19" s="97">
+        <f t="shared" si="2"/>
+        <v>5.2558330183999968E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -15704,8 +15952,20 @@
       <c r="R20" s="3">
         <v>4.92</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T20" s="97">
+        <f t="shared" si="0"/>
+        <v>0.10499755933333332</v>
+      </c>
+      <c r="U20" s="97">
+        <f t="shared" si="1"/>
+        <v>5.9776471000000012E-2</v>
+      </c>
+      <c r="V20" s="97">
+        <f t="shared" si="2"/>
+        <v>4.5221088333333312E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -15760,8 +16020,20 @@
       <c r="R21" s="3">
         <v>4.6210000000000004</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T21" s="97">
+        <f t="shared" si="0"/>
+        <v>8.0246297941333311E-2</v>
+      </c>
+      <c r="U21" s="97">
+        <f t="shared" si="1"/>
+        <v>5.0243409000000003E-2</v>
+      </c>
+      <c r="V21" s="97">
+        <f t="shared" si="2"/>
+        <v>3.0002888941333308E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -15816,8 +16088,20 @@
       <c r="R22" s="3">
         <v>4.4219999999999997</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T22" s="97">
+        <f t="shared" si="0"/>
+        <v>7.0273928149333337E-2</v>
+      </c>
+      <c r="U22" s="97">
+        <f t="shared" si="1"/>
+        <v>4.8228543999999998E-2</v>
+      </c>
+      <c r="V22" s="97">
+        <f t="shared" si="2"/>
+        <v>2.2045384149333339E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -15872,8 +16156,20 @@
       <c r="R23" s="3">
         <v>3.9249999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T23" s="97">
+        <f t="shared" si="0"/>
+        <v>4.9239458524666643E-2</v>
+      </c>
+      <c r="U23" s="97">
+        <f t="shared" si="1"/>
+        <v>3.810265212499999E-2</v>
+      </c>
+      <c r="V23" s="97">
+        <f t="shared" si="2"/>
+        <v>1.1136806399666653E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -15928,8 +16224,20 @@
       <c r="R24" s="3">
         <v>3.6190000000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T24" s="97">
+        <f t="shared" si="0"/>
+        <v>3.8441293506E-2</v>
+      </c>
+      <c r="U24" s="97">
+        <f t="shared" si="1"/>
+        <v>3.1704517125000005E-2</v>
+      </c>
+      <c r="V24" s="97">
+        <f t="shared" si="2"/>
+        <v>6.7367763809999953E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -15983,6 +16291,18 @@
       </c>
       <c r="R25" s="3">
         <v>2.8239999999999998</v>
+      </c>
+      <c r="T25" s="97">
+        <f t="shared" si="0"/>
+        <v>1.8266114005333331E-2</v>
+      </c>
+      <c r="U25" s="97">
+        <f t="shared" si="1"/>
+        <v>1.5438248999999999E-2</v>
+      </c>
+      <c r="V25" s="97">
+        <f t="shared" si="2"/>
+        <v>2.8278650053333316E-3</v>
       </c>
     </row>
   </sheetData>
@@ -16096,19 +16416,19 @@
       <c r="X1" s="107" t="s">
         <v>124</v>
       </c>
-      <c r="Z1" s="122" t="s">
+      <c r="Z1" s="117" t="s">
         <v>137</v>
       </c>
-      <c r="AA1" s="122"/>
-      <c r="AB1" s="122"/>
-      <c r="AD1" s="123" t="s">
+      <c r="AA1" s="117"/>
+      <c r="AB1" s="117"/>
+      <c r="AD1" s="118" t="s">
         <v>136</v>
       </c>
-      <c r="AE1" s="123"/>
-      <c r="AF1" s="123"/>
+      <c r="AE1" s="118"/>
+      <c r="AF1" s="118"/>
     </row>
     <row r="2" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="119" t="s">
         <v>153</v>
       </c>
       <c r="C2">
@@ -16199,7 +16519,7 @@
       </c>
     </row>
     <row r="3" spans="1:32" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="117"/>
+      <c r="B3" s="119"/>
       <c r="C3">
         <v>2</v>
       </c>
@@ -16290,10 +16610,10 @@
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="120" t="s">
         <v>146</v>
       </c>
-      <c r="B4" s="117"/>
+      <c r="B4" s="119"/>
       <c r="C4" s="102">
         <v>3</v>
       </c>
@@ -16384,7 +16704,7 @@
       </c>
     </row>
     <row r="5" spans="1:32" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="118"/>
+      <c r="A5" s="120"/>
       <c r="C5">
         <v>4</v>
       </c>
@@ -16479,7 +16799,7 @@
       </c>
     </row>
     <row r="6" spans="1:32" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="118"/>
+      <c r="A6" s="120"/>
       <c r="C6">
         <v>5</v>
       </c>
@@ -16574,7 +16894,7 @@
       </c>
     </row>
     <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="118"/>
+      <c r="A7" s="120"/>
       <c r="C7">
         <v>6</v>
       </c>
@@ -16668,7 +16988,7 @@
       </c>
     </row>
     <row r="8" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="118"/>
+      <c r="A8" s="120"/>
       <c r="C8">
         <v>7</v>
       </c>
@@ -16752,7 +17072,7 @@
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9" s="118"/>
+      <c r="A9" s="120"/>
       <c r="C9">
         <v>8</v>
       </c>
@@ -16826,7 +17146,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="118"/>
+      <c r="A10" s="120"/>
       <c r="C10">
         <v>9</v>
       </c>
@@ -16900,8 +17220,8 @@
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="118"/>
-      <c r="B11" s="119" t="s">
+      <c r="A11" s="120"/>
+      <c r="B11" s="121" t="s">
         <v>152</v>
       </c>
       <c r="C11" s="102">
@@ -16977,7 +17297,7 @@
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B12" s="119"/>
+      <c r="B12" s="121"/>
       <c r="C12">
         <v>11</v>
       </c>
@@ -17051,7 +17371,7 @@
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B13" s="119"/>
+      <c r="B13" s="121"/>
       <c r="C13">
         <v>12</v>
       </c>
@@ -17125,7 +17445,7 @@
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B14" s="119"/>
+      <c r="B14" s="121"/>
       <c r="C14">
         <v>13</v>
       </c>
@@ -17199,10 +17519,10 @@
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="120" t="s">
+      <c r="A15" s="122" t="s">
         <v>151</v>
       </c>
-      <c r="B15" s="119"/>
+      <c r="B15" s="121"/>
       <c r="C15" s="102">
         <v>14</v>
       </c>
@@ -17276,7 +17596,7 @@
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="120"/>
+      <c r="A16" s="122"/>
       <c r="C16">
         <v>15</v>
       </c>
@@ -17350,8 +17670,8 @@
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17" s="120"/>
-      <c r="B17" s="121" t="s">
+      <c r="A17" s="122"/>
+      <c r="B17" s="123" t="s">
         <v>147</v>
       </c>
       <c r="C17" s="102">
@@ -17424,7 +17744,7 @@
       </c>
     </row>
     <row r="18" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="121"/>
+      <c r="B18" s="123"/>
       <c r="C18">
         <v>17</v>
       </c>
@@ -17495,7 +17815,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B19" s="121"/>
+      <c r="B19" s="123"/>
       <c r="C19">
         <v>18</v>
       </c>
@@ -17566,7 +17886,7 @@
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B20" s="121"/>
+      <c r="B20" s="123"/>
       <c r="C20">
         <v>19</v>
       </c>
@@ -17637,7 +17957,7 @@
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B21" s="121"/>
+      <c r="B21" s="123"/>
       <c r="C21">
         <v>20</v>
       </c>
@@ -17708,7 +18028,7 @@
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B22" s="121"/>
+      <c r="B22" s="123"/>
       <c r="C22">
         <v>21</v>
       </c>
@@ -17779,7 +18099,7 @@
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B23" s="121"/>
+      <c r="B23" s="123"/>
       <c r="C23">
         <v>22</v>
       </c>
@@ -17850,7 +18170,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B24" s="121"/>
+      <c r="B24" s="123"/>
       <c r="C24">
         <v>23</v>
       </c>
@@ -17921,7 +18241,7 @@
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B25" s="121"/>
+      <c r="B25" s="123"/>
       <c r="C25">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
redesigned biplane spar to have same cross-sectional height as monoplane spar
</commit_message>
<xml_diff>
--- a/Sandia_blade_data.xlsx
+++ b/Sandia_blade_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24240" windowHeight="9465" tabRatio="793" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24240" windowHeight="9465" tabRatio="793" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Airfoil &amp; Chord Properties" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="twist vs. torsional stiffness" sheetId="6" r:id="rId6"/>
     <sheet name="monoplane_spar_layup" sheetId="7" r:id="rId7"/>
     <sheet name="biplane_spar_layup 20120306" sheetId="8" r:id="rId8"/>
+    <sheet name="biplane_spar_layup 20120517" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -459,7 +460,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="161">
   <si>
     <t>Station Number</t>
   </si>
@@ -1658,12 +1659,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="0.00000E+00"/>
     <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.00000"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -1970,7 +1972,7 @@
     <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2181,6 +2183,7 @@
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="20% - Accent1" xfId="6" builtinId="30"/>
@@ -2538,7 +2541,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2955,11 +2957,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43784832"/>
-        <c:axId val="43787008"/>
+        <c:axId val="104154240"/>
+        <c:axId val="104156160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43784832"/>
+        <c:axId val="104154240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2982,7 +2984,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -2999,12 +3000,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43787008"/>
+        <c:crossAx val="104156160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43787008"/>
+        <c:axId val="104156160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3026,7 +3027,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -3043,7 +3043,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43784832"/>
+        <c:crossAx val="104154240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3363,11 +3363,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43806720"/>
-        <c:axId val="43809024"/>
+        <c:axId val="104192256"/>
+        <c:axId val="104194816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43806720"/>
+        <c:axId val="104192256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3404,7 +3404,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -3435,12 +3434,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43809024"/>
+        <c:crossAx val="104194816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43809024"/>
+        <c:axId val="104194816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3466,7 +3465,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -3497,7 +3495,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43806720"/>
+        <c:crossAx val="104192256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1"/>
@@ -3550,7 +3548,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3967,11 +3964,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43868160"/>
-        <c:axId val="43870080"/>
+        <c:axId val="106146048"/>
+        <c:axId val="106152320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43868160"/>
+        <c:axId val="106146048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3994,7 +3991,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -4011,12 +4007,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43870080"/>
+        <c:crossAx val="106152320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43870080"/>
+        <c:axId val="106152320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4038,7 +4034,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -4055,7 +4050,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43868160"/>
+        <c:crossAx val="106146048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4375,11 +4370,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44094592"/>
-        <c:axId val="44096896"/>
+        <c:axId val="105913728"/>
+        <c:axId val="105932672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44094592"/>
+        <c:axId val="105913728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -4416,7 +4411,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -4447,12 +4441,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44096896"/>
+        <c:crossAx val="105932672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44096896"/>
+        <c:axId val="105932672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4478,7 +4472,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -4509,7 +4502,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44094592"/>
+        <c:crossAx val="105913728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1"/>
@@ -4781,8 +4774,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44719488"/>
-        <c:axId val="44725760"/>
+        <c:axId val="105968000"/>
+        <c:axId val="105969920"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4974,11 +4967,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44729856"/>
-        <c:axId val="44727680"/>
+        <c:axId val="105842944"/>
+        <c:axId val="105841024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44719488"/>
+        <c:axId val="105968000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -5045,12 +5038,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44725760"/>
+        <c:crossAx val="105969920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44725760"/>
+        <c:axId val="105969920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5114,12 +5107,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44719488"/>
+        <c:crossAx val="105968000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44727680"/>
+        <c:axId val="105841024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5193,13 +5186,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44729856"/>
+        <c:crossAx val="105842944"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2.0000000000000004E-2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44729856"/>
+        <c:axId val="105842944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5209,7 +5202,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44727680"/>
+        <c:crossAx val="105841024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5476,11 +5469,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44499328"/>
-        <c:axId val="44501632"/>
+        <c:axId val="105882368"/>
+        <c:axId val="105884672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44499328"/>
+        <c:axId val="105882368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -5517,7 +5510,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -5548,12 +5540,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44501632"/>
+        <c:crossAx val="105884672"/>
         <c:crossesAt val="-5.0000000000000012E-4"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44501632"/>
+        <c:axId val="105884672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5629,7 +5621,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44499328"/>
+        <c:crossAx val="105882368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6005,11 +5997,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44519808"/>
-        <c:axId val="44522880"/>
+        <c:axId val="105994496"/>
+        <c:axId val="106169856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44519808"/>
+        <c:axId val="105994496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.25"/>
@@ -6036,7 +6028,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
@@ -6055,12 +6046,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44522880"/>
+        <c:crossAx val="106169856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44522880"/>
+        <c:axId val="106169856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6098,7 +6089,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
@@ -6117,7 +6107,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44519808"/>
+        <c:crossAx val="105994496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6488,11 +6478,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44669184"/>
-        <c:axId val="44684800"/>
+        <c:axId val="106193664"/>
+        <c:axId val="106205184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44669184"/>
+        <c:axId val="106193664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0000000000000012E-2"/>
@@ -6520,7 +6510,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
@@ -6539,12 +6528,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44684800"/>
+        <c:crossAx val="106205184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44684800"/>
+        <c:axId val="106205184"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6583,7 +6572,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
@@ -6602,7 +6590,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44669184"/>
+        <c:crossAx val="106193664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14578,7 +14566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V2" sqref="V2:V25"/>
     </sheetView>
   </sheetViews>
@@ -14797,7 +14785,7 @@
         <v>5.8109999999999999</v>
       </c>
       <c r="T3" s="97">
-        <f t="shared" ref="T3:T26" si="0">(1/12)*$G$2*(J3+2*H3)^3</f>
+        <f t="shared" ref="T3:T25" si="0">(1/12)*$G$2*(J3+2*H3)^3</f>
         <v>21.636670572916664</v>
       </c>
       <c r="U3" s="97">
@@ -18444,4 +18432,1848 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="1.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="96" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="96" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="96" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="96" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="96" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="96" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="96" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="96" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="96" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" s="96" t="s">
+        <v>110</v>
+      </c>
+      <c r="K1" s="96" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" s="96" t="s">
+        <v>112</v>
+      </c>
+      <c r="M1" s="96" t="s">
+        <v>113</v>
+      </c>
+      <c r="N1" s="96" t="s">
+        <v>118</v>
+      </c>
+      <c r="O1" s="96" t="s">
+        <v>114</v>
+      </c>
+      <c r="P1" s="96" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q1" s="96" t="s">
+        <v>116</v>
+      </c>
+      <c r="R1" s="96" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" s="96" t="s">
+        <v>159</v>
+      </c>
+      <c r="U1" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="V1" s="96" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+      <c r="C2" s="98">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1.5</v>
+      </c>
+      <c r="F2" s="97">
+        <f>monoplane_spar_layup!F2/2</f>
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="G2" s="3">
+        <f>monoplane_spar_layup!G2-monoplane_spar_layup!I2</f>
+        <v>1.5859999999999999</v>
+      </c>
+      <c r="H2" s="124">
+        <f>0.5*(monoplane_spar_layup!H2*monoplane_spar_layup!G2)/(monoplane_spar_layup!G2-monoplane_spar_layup!I2)</f>
+        <v>3.3208070617906683E-2</v>
+      </c>
+      <c r="I2">
+        <f>K2+2*L2</f>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J2" s="3">
+        <v>5.266</v>
+      </c>
+      <c r="K2" s="3">
+        <f>monoplane_spar_layup!K2/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L2" s="97">
+        <f>monoplane_spar_layup!L2/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M2" s="3">
+        <v>13.308</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>2.4</v>
+      </c>
+      <c r="R2" s="3">
+        <v>5.7919999999999998</v>
+      </c>
+      <c r="T2" s="97">
+        <f>(1/12)*$G$2*(J2+2*H2)^3</f>
+        <v>20.039830322052929</v>
+      </c>
+      <c r="U2" s="97">
+        <f>(1/12)*$E$2*(J2-2*F2)^3</f>
+        <v>18.118916159625002</v>
+      </c>
+      <c r="V2" s="97">
+        <f>T2-U2</f>
+        <v>1.9209141624279269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="C3" s="98">
+        <v>2.1762800000000001E-3</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E3">
+        <v>1.5</v>
+      </c>
+      <c r="F3" s="97">
+        <f>monoplane_spar_layup!F3/2</f>
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="G3" s="3">
+        <f>monoplane_spar_layup!G3-monoplane_spar_layup!I3</f>
+        <v>1.5859999999999999</v>
+      </c>
+      <c r="H3" s="124">
+        <f>0.5*(monoplane_spar_layup!H3*monoplane_spar_layup!G3)/(monoplane_spar_layup!G3-monoplane_spar_layup!I3)</f>
+        <v>2.8991172761664567E-2</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I25" si="0">K3+2*L3</f>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J3" s="3">
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="K3" s="3">
+        <f>monoplane_spar_layup!K3/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L3" s="97">
+        <f>monoplane_spar_layup!L3/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M3" s="3">
+        <v>13.308</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>2.6</v>
+      </c>
+      <c r="R3" s="3">
+        <v>5.8109999999999999</v>
+      </c>
+      <c r="T3" s="97">
+        <f t="shared" ref="T3:T25" si="1">(1/12)*$G$2*(J3+2*H3)^3</f>
+        <v>19.933658523809985</v>
+      </c>
+      <c r="U3" s="97">
+        <f t="shared" ref="U3:U25" si="2">(1/12)*$E$2*(J3-2*F3)^3</f>
+        <v>18.108570375999999</v>
+      </c>
+      <c r="V3" s="97">
+        <f t="shared" ref="V3:V25" si="3">T3-U3</f>
+        <v>1.8250881478099856</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C4" s="98">
+        <v>2.5027199999999999E-2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="E4">
+        <v>1.5</v>
+      </c>
+      <c r="F4" s="97">
+        <f>monoplane_spar_layup!F4/2</f>
+        <v>0.01</v>
+      </c>
+      <c r="G4" s="3">
+        <f>monoplane_spar_layup!G4-monoplane_spar_layup!I4</f>
+        <v>1.5859999999999999</v>
+      </c>
+      <c r="H4" s="124">
+        <f>0.5*(monoplane_spar_layup!H4*monoplane_spar_layup!G4)/(monoplane_spar_layup!G4-monoplane_spar_layup!I4)</f>
+        <v>2.1084489281210594E-2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J4" s="3">
+        <v>5.0090000000000003</v>
+      </c>
+      <c r="K4" s="3">
+        <f>monoplane_spar_layup!K4/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L4" s="97">
+        <f>monoplane_spar_layup!L4/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M4" s="3">
+        <v>13.308</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>4.7</v>
+      </c>
+      <c r="R4" s="3">
+        <v>6.0579999999999998</v>
+      </c>
+      <c r="T4" s="97">
+        <f t="shared" si="1"/>
+        <v>17.033254249326692</v>
+      </c>
+      <c r="U4" s="97">
+        <f t="shared" si="2"/>
+        <v>15.522101708625007</v>
+      </c>
+      <c r="V4" s="97">
+        <f t="shared" si="3"/>
+        <v>1.5111525407016853</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C5" s="98">
+        <v>4.78781E-2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>4.8</v>
+      </c>
+      <c r="E5">
+        <v>1.5</v>
+      </c>
+      <c r="F5" s="97">
+        <f>monoplane_spar_layup!F5/2</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G5" s="3">
+        <f>monoplane_spar_layup!G5-monoplane_spar_layup!I5</f>
+        <v>1.5859999999999999</v>
+      </c>
+      <c r="H5" s="124">
+        <f>0.5*(monoplane_spar_layup!H5*monoplane_spar_layup!G5)/(monoplane_spar_layup!G5-monoplane_spar_layup!I5)</f>
+        <v>1.3177805800756623E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J5" s="3">
+        <v>4.7409999999999997</v>
+      </c>
+      <c r="K5" s="3">
+        <f>monoplane_spar_layup!K5/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L5" s="97">
+        <f>monoplane_spar_layup!L5/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M5" s="3">
+        <v>13.308</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>6.8</v>
+      </c>
+      <c r="R5" s="3">
+        <v>6.3040000000000003</v>
+      </c>
+      <c r="T5" s="97">
+        <f t="shared" si="1"/>
+        <v>14.32038131890471</v>
+      </c>
+      <c r="U5" s="97">
+        <f t="shared" si="2"/>
+        <v>13.069209678874994</v>
+      </c>
+      <c r="V5" s="97">
+        <f t="shared" si="3"/>
+        <v>1.2511716400297157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7">
+        <v>6.5</v>
+      </c>
+      <c r="C6" s="98">
+        <v>7.0729100000000003E-2</v>
+      </c>
+      <c r="D6" s="7">
+        <v>7.1</v>
+      </c>
+      <c r="E6">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="97">
+        <f>monoplane_spar_layup!F6/2</f>
+        <v>2.5499999999999998E-2</v>
+      </c>
+      <c r="G6" s="3">
+        <f>monoplane_spar_layup!G6-monoplane_spar_layup!I6</f>
+        <v>1.5859999999999999</v>
+      </c>
+      <c r="H6" s="124">
+        <f>0.5*(monoplane_spar_layup!H6*monoplane_spar_layup!G6)/(monoplane_spar_layup!G6-monoplane_spar_layup!I6)</f>
+        <v>7.9066834804539729E-3</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J6" s="3">
+        <v>4.4249999999999998</v>
+      </c>
+      <c r="K6" s="3">
+        <f>monoplane_spar_layup!K6/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L6" s="97">
+        <f>monoplane_spar_layup!L6/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M6" s="3">
+        <v>13.308</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>11</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>8.9</v>
+      </c>
+      <c r="R6" s="3">
+        <v>6.5510000000000002</v>
+      </c>
+      <c r="T6" s="97">
+        <f t="shared" si="1"/>
+        <v>11.574693552731265</v>
+      </c>
+      <c r="U6" s="97">
+        <f t="shared" si="2"/>
+        <v>10.460353202999999</v>
+      </c>
+      <c r="V6" s="97">
+        <f t="shared" si="3"/>
+        <v>1.1143403497312665</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7">
+        <v>9</v>
+      </c>
+      <c r="C7" s="98">
+        <v>9.7932500000000006E-2</v>
+      </c>
+      <c r="D7" s="7">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E7">
+        <v>1.5</v>
+      </c>
+      <c r="F7" s="97">
+        <f>monoplane_spar_layup!F7/2</f>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="G7" s="3">
+        <f>monoplane_spar_layup!G7-monoplane_spar_layup!I7</f>
+        <v>1.5859999999999999</v>
+      </c>
+      <c r="H7" s="124">
+        <f>0.5*(monoplane_spar_layup!H7*monoplane_spar_layup!G7)/(monoplane_spar_layup!G7-monoplane_spar_layup!I7)</f>
+        <v>2.6355611601513243E-3</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J7" s="3">
+        <v>4.0910000000000002</v>
+      </c>
+      <c r="K7" s="3">
+        <f>monoplane_spar_layup!K7/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L7" s="97">
+        <f>monoplane_spar_layup!L7/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M7" s="3">
+        <v>13.308</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>11.4</v>
+      </c>
+      <c r="R7" s="3">
+        <v>6.835</v>
+      </c>
+      <c r="T7" s="97">
+        <f t="shared" si="1"/>
+        <v>9.0842278453778835</v>
+      </c>
+      <c r="U7" s="97">
+        <f t="shared" si="2"/>
+        <v>8.1387950208750031</v>
+      </c>
+      <c r="V7" s="97">
+        <f t="shared" si="3"/>
+        <v>0.94543282450288046</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7">
+        <v>12.2</v>
+      </c>
+      <c r="C8" s="98">
+        <v>0.13275300000000001</v>
+      </c>
+      <c r="D8" s="7">
+        <v>13.3</v>
+      </c>
+      <c r="E8">
+        <v>1.5</v>
+      </c>
+      <c r="F8" s="97">
+        <f>monoplane_spar_layup!F8/2</f>
+        <v>4.7E-2</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J8" s="3">
+        <v>3.68</v>
+      </c>
+      <c r="K8" s="3">
+        <f>monoplane_spar_layup!K8/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L8" s="97">
+        <f>monoplane_spar_layup!L8/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M8" s="3">
+        <v>13.308</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>13</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>14.6</v>
+      </c>
+      <c r="R8" s="3">
+        <v>7.2149999999999999</v>
+      </c>
+      <c r="T8" s="97">
+        <f t="shared" si="1"/>
+        <v>6.5866622293333332</v>
+      </c>
+      <c r="U8" s="97">
+        <f t="shared" si="2"/>
+        <v>5.7642242570000013</v>
+      </c>
+      <c r="V8" s="97">
+        <f t="shared" si="3"/>
+        <v>0.82243797233333193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7">
+        <v>13.9</v>
+      </c>
+      <c r="C9" s="98">
+        <v>0.151251</v>
+      </c>
+      <c r="D9" s="7">
+        <v>15.1</v>
+      </c>
+      <c r="E9">
+        <v>1.5</v>
+      </c>
+      <c r="F9" s="97">
+        <f>monoplane_spar_layup!F9/2</f>
+        <v>5.5500000000000001E-2</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J9" s="3">
+        <v>3.48</v>
+      </c>
+      <c r="K9" s="3">
+        <f>monoplane_spar_layup!K9/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L9" s="97">
+        <f>monoplane_spar_layup!L9/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M9" s="3">
+        <v>13.177</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="O9">
+        <v>-1.34E-3</v>
+      </c>
+      <c r="P9">
+        <v>14</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>16.3</v>
+      </c>
+      <c r="R9" s="3">
+        <v>7.4039999999999999</v>
+      </c>
+      <c r="T9" s="97">
+        <f t="shared" si="1"/>
+        <v>5.5700573760000003</v>
+      </c>
+      <c r="U9" s="97">
+        <f t="shared" si="2"/>
+        <v>4.7798365511249985</v>
+      </c>
+      <c r="V9" s="97">
+        <f t="shared" si="3"/>
+        <v>0.79022082487500178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7">
+        <v>15.5</v>
+      </c>
+      <c r="C10" s="98">
+        <v>0.16866200000000001</v>
+      </c>
+      <c r="D10" s="7">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="E10">
+        <v>1.5</v>
+      </c>
+      <c r="F10" s="97">
+        <f>monoplane_spar_layup!F10/2</f>
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J10" s="3">
+        <v>3.2850000000000001</v>
+      </c>
+      <c r="K10" s="3">
+        <f>monoplane_spar_layup!K10/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L10" s="97">
+        <f>monoplane_spar_layup!L10/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M10" s="3">
+        <v>13.045999999999999</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="O10">
+        <v>-1.4300000000000001E-3</v>
+      </c>
+      <c r="P10">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="R10" s="3">
+        <v>7.5519999999999996</v>
+      </c>
+      <c r="T10" s="97">
+        <f t="shared" si="1"/>
+        <v>4.6851991801875004</v>
+      </c>
+      <c r="U10" s="97">
+        <f t="shared" si="2"/>
+        <v>3.9668222870000016</v>
+      </c>
+      <c r="V10" s="97">
+        <f t="shared" si="3"/>
+        <v>0.71837689318749876</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="C11" s="98">
+        <v>0.18607199999999999</v>
+      </c>
+      <c r="D11" s="7">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E11">
+        <v>1.5</v>
+      </c>
+      <c r="F11" s="97">
+        <f>monoplane_spar_layup!F11/2</f>
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J11" s="3">
+        <v>3.089</v>
+      </c>
+      <c r="K11" s="3">
+        <f>monoplane_spar_layup!K11/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L11" s="97">
+        <f>monoplane_spar_layup!L11/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M11" s="3">
+        <v>12.914999999999999</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="O11">
+        <v>-1.4300000000000001E-3</v>
+      </c>
+      <c r="P11">
+        <v>16</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>19.5</v>
+      </c>
+      <c r="R11" s="3">
+        <v>7.6280000000000001</v>
+      </c>
+      <c r="T11" s="97">
+        <f t="shared" si="1"/>
+        <v>3.895611702902833</v>
+      </c>
+      <c r="U11" s="97">
+        <f t="shared" si="2"/>
+        <v>3.2188471471249995</v>
+      </c>
+      <c r="V11" s="97">
+        <f t="shared" si="3"/>
+        <v>0.67676455577783345</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7">
+        <v>19.8</v>
+      </c>
+      <c r="C12" s="98">
+        <v>0.215452</v>
+      </c>
+      <c r="D12" s="7">
+        <v>21.5</v>
+      </c>
+      <c r="E12">
+        <v>1.5</v>
+      </c>
+      <c r="F12" s="97">
+        <f>monoplane_spar_layup!F12/2</f>
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J12" s="3">
+        <v>2.8820000000000001</v>
+      </c>
+      <c r="K12" s="3">
+        <f>monoplane_spar_layup!K12/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L12" s="97">
+        <f>monoplane_spar_layup!L12/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M12" s="3">
+        <v>12.132999999999999</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="O12">
+        <v>-5.0499999999999998E-3</v>
+      </c>
+      <c r="P12">
+        <v>17</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>22.2</v>
+      </c>
+      <c r="R12" s="3">
+        <v>7.585</v>
+      </c>
+      <c r="T12" s="97">
+        <f t="shared" si="1"/>
+        <v>3.1637624439373337</v>
+      </c>
+      <c r="U12" s="97">
+        <f t="shared" si="2"/>
+        <v>2.5882821169999999</v>
+      </c>
+      <c r="V12" s="97">
+        <f t="shared" si="3"/>
+        <v>0.57548032693733386</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7">
+        <v>22.5</v>
+      </c>
+      <c r="C13" s="98">
+        <v>0.24483099999999999</v>
+      </c>
+      <c r="D13" s="7">
+        <v>24.5</v>
+      </c>
+      <c r="E13">
+        <v>1.5</v>
+      </c>
+      <c r="F13" s="97">
+        <f>monoplane_spar_layup!F13/2</f>
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J13" s="3">
+        <v>2.6960000000000002</v>
+      </c>
+      <c r="K13" s="3">
+        <f>monoplane_spar_layup!K13/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L13" s="97">
+        <f>monoplane_spar_layup!L13/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M13" s="3">
+        <v>11.35</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="O13">
+        <v>-5.0600000000000003E-3</v>
+      </c>
+      <c r="P13">
+        <v>18</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>24.9</v>
+      </c>
+      <c r="R13" s="3">
+        <v>7.4880000000000004</v>
+      </c>
+      <c r="T13" s="97">
+        <f t="shared" si="1"/>
+        <v>2.5898916803413337</v>
+      </c>
+      <c r="U13" s="97">
+        <f t="shared" si="2"/>
+        <v>2.0971520000000003</v>
+      </c>
+      <c r="V13" s="97">
+        <f t="shared" si="3"/>
+        <v>0.49273968034133331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7">
+        <v>25.2</v>
+      </c>
+      <c r="C14" s="98">
+        <v>0.27421099999999998</v>
+      </c>
+      <c r="D14" s="7">
+        <v>27.4</v>
+      </c>
+      <c r="E14">
+        <v>1.5</v>
+      </c>
+      <c r="F14" s="97">
+        <f>monoplane_spar_layup!F14/2</f>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J14" s="3">
+        <v>2.4980000000000002</v>
+      </c>
+      <c r="K14" s="3">
+        <f>monoplane_spar_layup!K14/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L14" s="97">
+        <f>monoplane_spar_layup!L14/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M14" s="3">
+        <v>10.568</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0.184</v>
+      </c>
+      <c r="O14">
+        <v>-5.0499999999999998E-3</v>
+      </c>
+      <c r="P14">
+        <v>19</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>27.6</v>
+      </c>
+      <c r="R14" s="3">
+        <v>7.3470000000000004</v>
+      </c>
+      <c r="T14" s="97">
+        <f t="shared" si="1"/>
+        <v>2.0601518806093337</v>
+      </c>
+      <c r="U14" s="97">
+        <f t="shared" si="2"/>
+        <v>1.6640066250000001</v>
+      </c>
+      <c r="V14" s="97">
+        <f t="shared" si="3"/>
+        <v>0.39614525560933367</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7">
+        <v>33.4</v>
+      </c>
+      <c r="C15" s="98">
+        <v>0.36343900000000001</v>
+      </c>
+      <c r="D15" s="7">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="E15">
+        <v>1.5</v>
+      </c>
+      <c r="F15" s="97">
+        <f>monoplane_spar_layup!F15/2</f>
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J15" s="3">
+        <v>2.077</v>
+      </c>
+      <c r="K15" s="3">
+        <f>monoplane_spar_layup!K15/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L15" s="97">
+        <f>monoplane_spar_layup!L15/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M15" s="3">
+        <v>9.1660000000000004</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="O15">
+        <v>-2.98E-3</v>
+      </c>
+      <c r="P15">
+        <v>20</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="R15" s="3">
+        <v>6.923</v>
+      </c>
+      <c r="T15" s="97">
+        <f t="shared" si="1"/>
+        <v>1.1842173687781665</v>
+      </c>
+      <c r="U15" s="97">
+        <f t="shared" si="2"/>
+        <v>0.93831373899999992</v>
+      </c>
+      <c r="V15" s="97">
+        <f t="shared" si="3"/>
+        <v>0.2459036297781666</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7">
+        <v>41.5</v>
+      </c>
+      <c r="C16" s="98">
+        <v>0.45157799999999998</v>
+      </c>
+      <c r="D16" s="7">
+        <v>45.2</v>
+      </c>
+      <c r="E16">
+        <v>1.5</v>
+      </c>
+      <c r="F16" s="97">
+        <f>monoplane_spar_layup!F16/2</f>
+        <v>5.5500000000000001E-2</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J16" s="3">
+        <v>1.6719999999999999</v>
+      </c>
+      <c r="K16" s="3">
+        <f>monoplane_spar_layup!K16/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L16" s="97">
+        <f>monoplane_spar_layup!L16/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M16" s="3">
+        <v>7.6879999999999997</v>
+      </c>
+      <c r="N16" s="3">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="O16">
+        <v>-3.1800000000000001E-3</v>
+      </c>
+      <c r="P16">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>43.9</v>
+      </c>
+      <c r="R16" s="3">
+        <v>6.4290000000000003</v>
+      </c>
+      <c r="T16" s="97">
+        <f t="shared" si="1"/>
+        <v>0.61777560721066649</v>
+      </c>
+      <c r="U16" s="97">
+        <f t="shared" si="2"/>
+        <v>0.47546518512499997</v>
+      </c>
+      <c r="V16" s="97">
+        <f t="shared" si="3"/>
+        <v>0.14231042208566652</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7">
+        <v>49.6</v>
+      </c>
+      <c r="C17" s="98">
+        <v>0.539717</v>
+      </c>
+      <c r="D17" s="7">
+        <v>54</v>
+      </c>
+      <c r="E17">
+        <v>1.5</v>
+      </c>
+      <c r="F17" s="97">
+        <f>monoplane_spar_layup!F17/2</f>
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1.36</v>
+      </c>
+      <c r="K17" s="3">
+        <f>monoplane_spar_layup!K17/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L17" s="97">
+        <f>monoplane_spar_layup!L17/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M17" s="3">
+        <v>6.18</v>
+      </c>
+      <c r="N17" s="3">
+        <v>0.108</v>
+      </c>
+      <c r="O17">
+        <v>-3.2499999999999999E-3</v>
+      </c>
+      <c r="P17">
+        <v>22</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>52</v>
+      </c>
+      <c r="R17" s="3">
+        <v>5.915</v>
+      </c>
+      <c r="T17" s="97">
+        <f t="shared" si="1"/>
+        <v>0.33245943466666672</v>
+      </c>
+      <c r="U17" s="97">
+        <f t="shared" si="2"/>
+        <v>0.24885818900000001</v>
+      </c>
+      <c r="V17" s="97">
+        <f t="shared" si="3"/>
+        <v>8.3601245666666713E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7">
+        <v>57.8</v>
+      </c>
+      <c r="C18" s="98">
+        <v>0.62894499999999998</v>
+      </c>
+      <c r="D18" s="7">
+        <v>62.9</v>
+      </c>
+      <c r="E18">
+        <v>1.5</v>
+      </c>
+      <c r="F18" s="97">
+        <f>monoplane_spar_layup!F18/2</f>
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="K18" s="3">
+        <f>monoplane_spar_layup!K18/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L18" s="97">
+        <f>monoplane_spar_layup!L18/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M18" s="3">
+        <v>4.7430000000000003</v>
+      </c>
+      <c r="N18" s="3">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="O18">
+        <v>-3.0599999999999998E-3</v>
+      </c>
+      <c r="P18">
+        <v>23</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>60.2</v>
+      </c>
+      <c r="R18" s="3">
+        <v>5.4169999999999998</v>
+      </c>
+      <c r="T18" s="97">
+        <f t="shared" si="1"/>
+        <v>0.19478195618266661</v>
+      </c>
+      <c r="U18" s="97">
+        <f t="shared" si="2"/>
+        <v>0.14594698462499997</v>
+      </c>
+      <c r="V18" s="97">
+        <f t="shared" si="3"/>
+        <v>4.883497155766664E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7">
+        <v>64.3</v>
+      </c>
+      <c r="C19" s="98">
+        <v>0.69967400000000002</v>
+      </c>
+      <c r="D19" s="7">
+        <v>70</v>
+      </c>
+      <c r="E19">
+        <v>1.5</v>
+      </c>
+      <c r="F19" s="97">
+        <f>monoplane_spar_layup!F19/2</f>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="K19" s="3">
+        <f>monoplane_spar_layup!K19/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L19" s="97">
+        <f>monoplane_spar_layup!L19/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M19" s="3">
+        <v>3.633</v>
+      </c>
+      <c r="N19" s="3">
+        <v>6.3E-2</v>
+      </c>
+      <c r="O19">
+        <v>-2.98E-3</v>
+      </c>
+      <c r="P19">
+        <v>24</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>66.7</v>
+      </c>
+      <c r="R19" s="3">
+        <v>5.0190000000000001</v>
+      </c>
+      <c r="T19" s="97">
+        <f t="shared" si="1"/>
+        <v>0.11475379609199997</v>
+      </c>
+      <c r="U19" s="97">
+        <f t="shared" si="2"/>
+        <v>8.6938306999999965E-2</v>
+      </c>
+      <c r="V19" s="97">
+        <f t="shared" si="3"/>
+        <v>2.7815489092000004E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="C20" s="98">
+        <v>0.71708400000000005</v>
+      </c>
+      <c r="D20" s="7">
+        <v>71.7</v>
+      </c>
+      <c r="E20">
+        <v>1.5</v>
+      </c>
+      <c r="F20" s="97">
+        <f>monoplane_spar_layup!F20/2</f>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="K20" s="3">
+        <f>monoplane_spar_layup!K20/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L20" s="97">
+        <f>monoplane_spar_layup!L20/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M20" s="3">
+        <v>3.383</v>
+      </c>
+      <c r="N20" s="3">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="O20">
+        <v>-2.7299999999999998E-3</v>
+      </c>
+      <c r="P20">
+        <v>25</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>68.3</v>
+      </c>
+      <c r="R20" s="3">
+        <v>4.92</v>
+      </c>
+      <c r="T20" s="97">
+        <f t="shared" si="1"/>
+        <v>9.9596967166666675E-2</v>
+      </c>
+      <c r="U20" s="97">
+        <f t="shared" si="2"/>
+        <v>7.5686967000000022E-2</v>
+      </c>
+      <c r="V20" s="97">
+        <f t="shared" si="3"/>
+        <v>2.3910000166666653E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7">
+        <v>70.8</v>
+      </c>
+      <c r="C21" s="98">
+        <v>0.77040299999999995</v>
+      </c>
+      <c r="D21" s="7">
+        <v>77</v>
+      </c>
+      <c r="E21">
+        <v>1.5</v>
+      </c>
+      <c r="F21" s="97">
+        <f>monoplane_spar_layup!F21/2</f>
+        <v>2.35E-2</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="K21" s="3">
+        <f>monoplane_spar_layup!K21/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L21" s="97">
+        <f>monoplane_spar_layup!L21/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M21" s="3">
+        <v>2.7349999999999999</v>
+      </c>
+      <c r="N21" s="3">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="O21">
+        <v>-2.31E-3</v>
+      </c>
+      <c r="P21">
+        <v>26</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>73.2</v>
+      </c>
+      <c r="R21" s="3">
+        <v>4.6210000000000004</v>
+      </c>
+      <c r="T21" s="97">
+        <f t="shared" si="1"/>
+        <v>7.6118796970666661E-2</v>
+      </c>
+      <c r="U21" s="97">
+        <f t="shared" si="2"/>
+        <v>6.0467078124999983E-2</v>
+      </c>
+      <c r="V21" s="97">
+        <f t="shared" si="3"/>
+        <v>1.5651718845666678E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7">
+        <v>74</v>
+      </c>
+      <c r="C22" s="98">
+        <v>0.80522300000000002</v>
+      </c>
+      <c r="D22" s="7">
+        <v>80.5</v>
+      </c>
+      <c r="E22">
+        <v>1.5</v>
+      </c>
+      <c r="F22" s="97">
+        <f>monoplane_spar_layup!F22/2</f>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="K22" s="3">
+        <f>monoplane_spar_layup!K22/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L22" s="97">
+        <f>monoplane_spar_layup!L22/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M22" s="3">
+        <v>2.3479999999999999</v>
+      </c>
+      <c r="N22" s="3">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="O22">
+        <v>-2.1099999999999999E-3</v>
+      </c>
+      <c r="P22">
+        <v>27</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="R22" s="3">
+        <v>4.4219999999999997</v>
+      </c>
+      <c r="T22" s="97">
+        <f t="shared" si="1"/>
+        <v>6.6659360074666676E-2</v>
+      </c>
+      <c r="U22" s="97">
+        <f t="shared" si="2"/>
+        <v>5.5306341000000009E-2</v>
+      </c>
+      <c r="V22" s="97">
+        <f t="shared" si="3"/>
+        <v>1.1353019074666668E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7">
+        <v>82.2</v>
+      </c>
+      <c r="C23" s="98">
+        <v>0.89444999999999997</v>
+      </c>
+      <c r="D23" s="7">
+        <v>89.4</v>
+      </c>
+      <c r="E23">
+        <v>1.5</v>
+      </c>
+      <c r="F23" s="97">
+        <f>monoplane_spar_layup!F23/2</f>
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="K23" s="3">
+        <f>monoplane_spar_layup!K23/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L23" s="97">
+        <f>monoplane_spar_layup!L23/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M23" s="3">
+        <v>1.38</v>
+      </c>
+      <c r="N23" s="3">
+        <v>2.4E-2</v>
+      </c>
+      <c r="O23">
+        <v>-2.0600000000000002E-3</v>
+      </c>
+      <c r="P23">
+        <v>28</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>84.6</v>
+      </c>
+      <c r="R23" s="3">
+        <v>3.9249999999999998</v>
+      </c>
+      <c r="T23" s="97">
+        <f t="shared" si="1"/>
+        <v>4.670680694983332E-2</v>
+      </c>
+      <c r="U23" s="97">
+        <f t="shared" si="2"/>
+        <v>4.1063624999999992E-2</v>
+      </c>
+      <c r="V23" s="97">
+        <f t="shared" si="3"/>
+        <v>5.6431819498333272E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7">
+        <v>87</v>
+      </c>
+      <c r="C24" s="98">
+        <v>0.94668099999999999</v>
+      </c>
+      <c r="D24" s="7">
+        <v>94.7</v>
+      </c>
+      <c r="E24">
+        <v>1.5</v>
+      </c>
+      <c r="F24" s="97">
+        <f>monoplane_spar_layup!F24/2</f>
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="K24" s="3">
+        <f>monoplane_spar_layup!K24/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L24" s="97">
+        <f>monoplane_spar_layup!L24/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M24" s="3">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="N24" s="3">
+        <v>1.4E-2</v>
+      </c>
+      <c r="O24">
+        <v>-2.1099999999999999E-3</v>
+      </c>
+      <c r="P24">
+        <v>29</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>89.4</v>
+      </c>
+      <c r="R24" s="3">
+        <v>3.6190000000000002</v>
+      </c>
+      <c r="T24" s="97">
+        <f t="shared" si="1"/>
+        <v>3.6464049940500003E-2</v>
+      </c>
+      <c r="U24" s="97">
+        <f t="shared" si="2"/>
+        <v>3.3076161E-2</v>
+      </c>
+      <c r="V24" s="97">
+        <f t="shared" si="3"/>
+        <v>3.3878889405000029E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7">
+        <v>91.9</v>
+      </c>
+      <c r="C25" s="98">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7">
+        <v>100</v>
+      </c>
+      <c r="E25">
+        <v>1.5</v>
+      </c>
+      <c r="F25" s="97">
+        <f>monoplane_spar_layup!F25/2</f>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000003E-2</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="K25" s="3">
+        <f>monoplane_spar_layup!K25/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="L25" s="97">
+        <f>monoplane_spar_layup!L25/2</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="N25" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="O25">
+        <v>-1.8500000000000001E-3</v>
+      </c>
+      <c r="P25">
+        <v>30</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>94.3</v>
+      </c>
+      <c r="R25" s="3">
+        <v>2.8239999999999998</v>
+      </c>
+      <c r="T25" s="97">
+        <f t="shared" si="1"/>
+        <v>1.7326589002666665E-2</v>
+      </c>
+      <c r="U25" s="97">
+        <f t="shared" si="2"/>
+        <v>1.5907940874999998E-2</v>
+      </c>
+      <c r="V25" s="97">
+        <f t="shared" si="3"/>
+        <v>1.418648127666667E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>